<commit_message>
Change the colors in the plots.
Add a new poster file to avoid conflicts where I added a new chart.
</commit_message>
<xml_diff>
--- a/Frequency_table_clades.xlsx
+++ b/Frequency_table_clades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\VM Shared Folder\Github\DataVis\DataVis2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70282D00-790D-49BF-81D6-10CDF5B0E913}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFD7A20-93F4-44FB-9196-7944B628F63A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{24388B20-B62C-40D3-9705-EF5AA6AD371B}"/>
   </bookViews>
@@ -93,6 +93,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="[$-409]mmm\-yy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -130,16 +133,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD1D1D1"/>
+      <color rgb="FFC35944"/>
+      <color rgb="FF934BC9"/>
+      <color rgb="FFB381D9"/>
+      <color rgb="FF3183A8"/>
+      <color rgb="FFAABF55"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6488,7 +6502,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6501,22 +6515,22 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" b="1"/>
               <a:t>Estimated</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
               <a:t> d</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" b="1"/>
               <a:t>istribution</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of strains on Active Worldwide Cases</a:t>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> of Variants on Active Worldwide Cases</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6533,7 +6547,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -6572,7 +6586,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="25000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6584,7 +6600,7 @@
             <c:numRef>
               <c:f>'Stacked bar Total Cases'!$L$1:$S$1</c:f>
               <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -6668,7 +6684,10 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6680,7 +6699,7 @@
             <c:numRef>
               <c:f>'Stacked bar Total Cases'!$L$1:$S$1</c:f>
               <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -6764,7 +6783,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:schemeClr val="bg2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6776,7 +6795,7 @@
             <c:numRef>
               <c:f>'Stacked bar Total Cases'!$L$1:$S$1</c:f>
               <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -6860,8 +6879,8 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="90000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -6874,7 +6893,7 @@
             <c:numRef>
               <c:f>'Stacked bar Total Cases'!$L$1:$S$1</c:f>
               <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -6958,8 +6977,8 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4">
-                <a:lumMod val="60000"/>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -6972,7 +6991,7 @@
             <c:numRef>
               <c:f>'Stacked bar Total Cases'!$L$1:$S$1</c:f>
               <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -7056,9 +7075,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
+              <a:srgbClr val="B381D9"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -7070,7 +7087,7 @@
             <c:numRef>
               <c:f>'Stacked bar Total Cases'!$L$1:$S$1</c:f>
               <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -7154,10 +7171,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="80000"/>
-                <a:lumOff val="20000"/>
-              </a:schemeClr>
+              <a:srgbClr val="934BC9"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -7169,7 +7183,7 @@
             <c:numRef>
               <c:f>'Stacked bar Total Cases'!$L$1:$S$1</c:f>
               <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -7254,8 +7268,8 @@
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent4">
-                <a:lumMod val="80000"/>
-                <a:lumOff val="20000"/>
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -7268,7 +7282,7 @@
             <c:numRef>
               <c:f>'Stacked bar Total Cases'!$L$1:$S$1</c:f>
               <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -7352,9 +7366,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="80000"/>
-                <a:lumOff val="20000"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -7367,7 +7381,7 @@
             <c:numRef>
               <c:f>'Stacked bar Total Cases'!$L$1:$S$1</c:f>
               <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -7451,9 +7465,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="80000"/>
-              </a:schemeClr>
+              <a:srgbClr val="AABF55"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -7465,7 +7477,7 @@
             <c:numRef>
               <c:f>'Stacked bar Total Cases'!$L$1:$S$1</c:f>
               <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -7549,9 +7561,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4">
-                <a:lumMod val="80000"/>
-              </a:schemeClr>
+              <a:srgbClr val="3183A8"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -7563,7 +7573,7 @@
             <c:numRef>
               <c:f>'Stacked bar Total Cases'!$L$1:$S$1</c:f>
               <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -7647,9 +7657,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="80000"/>
-              </a:schemeClr>
+              <a:srgbClr val="C35944"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -7661,7 +7669,7 @@
             <c:numRef>
               <c:f>'Stacked bar Total Cases'!$L$1:$S$1</c:f>
               <c:numCache>
-                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -7806,7 +7814,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:numFmt formatCode="[$-409]mmm\-yy;@" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7828,7 +7836,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -7946,7 +7954,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8024,14 +8032,17 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:srgbClr val="D1D1D1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
-    <a:effectLst/>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+        <a:prstClr val="black">
+          <a:alpha val="40000"/>
+        </a:prstClr>
+      </a:outerShdw>
+    </a:effectLst>
   </c:spPr>
   <c:txPr>
     <a:bodyPr/>
@@ -9762,226 +9773,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Connector 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{418D850C-7C5C-442D-B5BA-81B7A0A9C502}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="11910060" y="3535680"/>
-          <a:ext cx="533400" cy="670560"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Connector 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{574E949B-0F54-4FA2-B58D-20FED0650B21}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="11910060" y="3733800"/>
-          <a:ext cx="510540" cy="487680"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="Straight Connector 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2438B55B-29F1-4A4A-803A-5270986D95E3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12961620" y="3741420"/>
-          <a:ext cx="548640" cy="502920"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="Straight Connector 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5843149-3B0C-4153-8BDA-96603C9F3ADE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="12961620" y="3489960"/>
-          <a:ext cx="556260" cy="53340"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>14</xdr:row>
@@ -11223,8 +11014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EBEE6B8-6449-4BD3-9780-821FDD19DB72}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F14" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView tabSelected="1" topLeftCell="I13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W31" sqref="W31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -11260,28 +11051,28 @@
       <c r="K1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L1" s="3">
         <v>43831</v>
       </c>
-      <c r="M1" s="1">
+      <c r="M1" s="3">
         <v>43891</v>
       </c>
-      <c r="N1" s="1">
+      <c r="N1" s="3">
         <v>43952</v>
       </c>
-      <c r="O1" s="1">
+      <c r="O1" s="3">
         <v>44013</v>
       </c>
-      <c r="P1" s="1">
+      <c r="P1" s="3">
         <v>44075</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="Q1" s="3">
         <v>44136</v>
       </c>
-      <c r="R1" s="1">
+      <c r="R1" s="3">
         <v>44197</v>
       </c>
-      <c r="S1" s="1">
+      <c r="S1" s="3">
         <v>44256</v>
       </c>
     </row>
@@ -12137,6 +11928,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Worked on charts for the bottom of the poster.
use Map Data and frequency clades excel, in poster post crash with charts below .svg.
</commit_message>
<xml_diff>
--- a/Frequency_table_clades.xlsx
+++ b/Frequency_table_clades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\VM Shared Folder\Github\DataVis\DataVis2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE652E8B-CE09-41F2-A37A-FCD70C449B08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61EB44F-59BA-4D1F-9792-C96D65C7C354}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{24388B20-B62C-40D3-9705-EF5AA6AD371B}"/>
   </bookViews>
@@ -156,16 +156,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE41C8E"/>
+      <color rgb="FFB381D9"/>
+      <color rgb="FF652B91"/>
       <color rgb="FFFF9900"/>
       <color rgb="FF6C7A2E"/>
       <color rgb="FF753225"/>
       <color rgb="FF296D8B"/>
       <color rgb="FFFF9933"/>
-      <color rgb="FFB381D9"/>
       <color rgb="FF934BC9"/>
       <color rgb="FFAF2387"/>
-      <color rgb="FFF6D250"/>
-      <color rgb="FFAABF55"/>
     </mruColors>
   </colors>
   <extLst>
@@ -8129,7 +8129,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.5495723108078871E-2"/>
+          <c:y val="0.12494999836023624"/>
+          <c:w val="0.7542457285527483"/>
+          <c:h val="0.78611711806018747"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -9695,66 +9705,11 @@
         <c:axId val="899350543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="44287"/>
-          <c:min val="43946"/>
+          <c:max val="44256"/>
+          <c:min val="43976"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="[$-409]mmm\-yy;@" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -9777,7 +9732,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -9794,7 +9749,7 @@
         </c:txPr>
         <c:crossAx val="899360111"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="0"/>
+        <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
         <c:majorUnit val="1"/>
@@ -9830,7 +9785,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -9843,10 +9798,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
                   <a:t>Cases (in Millions)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1100" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -9863,7 +9818,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -9911,8 +9866,8 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="899350543"/>
-        <c:crossesAt val="43891"/>
-        <c:crossBetween val="midCat"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
         </c:dispUnits>
@@ -9927,6 +9882,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="tr"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.85414165026246724"/>
+          <c:y val="0.13770209588471208"/>
+          <c:w val="7.6499412756373827E-2"/>
+          <c:h val="0.77944210328937091"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9968,24 +9933,1857 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="bg2">
-          <a:lumMod val="10000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
-    <a:effectLst>
-      <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-        <a:prstClr val="black">
-          <a:alpha val="40000"/>
-        </a:prstClr>
-      </a:outerShdw>
-    </a:effectLst>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.4193631069553808E-2"/>
+          <c:y val="9.7022872455797882E-2"/>
+          <c:w val="0.7542457285527483"/>
+          <c:h val="0.78611711806018747"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked bar Total Cases'!$A$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>19A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$63:$P$63</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$64:$P$64</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$64:$P$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>172931.28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87570.72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>121018.65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116837.26000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>130144.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72970.64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>115585.90000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F9B0-4CDD-A591-1B6307592045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked bar Total Cases'!$A$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>19B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$63:$P$63</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$65:$P$65</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$65:$P$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>151314.87000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116760.96000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80679.100000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116837.26000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>130144.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72970.64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600849.44999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>226513.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>205193.28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F9B0-4CDD-A591-1B6307592045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked bar Total Cases'!$A$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F6D250"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$63:$P$63</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$66:$P$66</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$66:$P$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>951122.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1196799.8399999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1694261.0999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1986233.4200000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2147377.65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2116148.56</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3698748.8000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5594346.1200000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5607928.2000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5889361.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4309058.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F9B0-4CDD-A591-1B6307592045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked bar Total Cases'!$A$67</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$63:$P$63</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$67:$P$67</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$67:$P$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>518793.83999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1050848.6399999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1532902.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2570419.7200000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2863170.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3283678.8000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4970193.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6441974.3200000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5808211.3499999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5889361.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4309058.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F9B0-4CDD-A591-1B6307592045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked bar Total Cases'!$A$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF9900"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$63:$P$63</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$68:$P$68</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$68:$P$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>345862.56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>379473.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>443735.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>408930.41000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>585648.44999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>656735.76</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>809101.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1356205.12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1802548.3499999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>906055.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1846739.52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F9B0-4CDD-A591-1B6307592045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked bar Total Cases'!$A$69</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="AF2387"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$63:$P$63</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$69:$P$69</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$69:$P$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>21616.41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58380.480000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80679.100000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>175255.88999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>195216.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>364853.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>577929.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>508576.92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>801132.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>906055.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>205193.28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-F9B0-4CDD-A591-1B6307592045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked bar Total Cases'!$A$70</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20E(EU1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="934BC9"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$63:$P$63</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$70:$P$70</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$70:$P$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58418.630000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65072.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>291882.56</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>809101.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1525730.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>801132.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1132569.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1025966.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-F9B0-4CDD-A591-1B6307592045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked bar Total Cases'!$A$71</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20F</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E41C8E"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$63:$P$63</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$71:$P$71</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$71:$P$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80679.100000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>350511.77999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>260288.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>291882.56</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>231171.80000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-F9B0-4CDD-A591-1B6307592045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked bar Total Cases'!$A$72</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20G</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="652B91"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$63:$P$63</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$72:$P$72</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$72:$P$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29190.240000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58418.630000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>130144.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>145941.28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>346757.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>847628.20000000007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1001415.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1132569.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1641546.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-F9B0-4CDD-A591-1B6307592045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked bar Total Cases'!$A$73</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20H(ZA)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="6C7A2E"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$63:$P$63</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$73:$P$73</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$73:$P$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>678102.56</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1802548.3499999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2038625.0999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>410386.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-F9B0-4CDD-A591-1B6307592045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked bar Total Cases'!$A$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20I(UK)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="296D8B"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$63:$P$63</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$74:$P$74</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$74:$P$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1602265.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3850736.3000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5745411.8400000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-F9B0-4CDD-A591-1B6307592045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked bar Total Cases'!$A$75</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20J(BR)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="753225"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$63:$P$63</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Stacked bar Total Cases'!$B$75:$P$75</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Stacked bar Total Cases'!$F$75:$P$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200283.15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>679541.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>820773.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-F9B0-4CDD-A591-1B6307592045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="24"/>
+        <c:overlap val="100"/>
+        <c:axId val="899350543"/>
+        <c:axId val="899360111"/>
+      </c:barChart>
+      <c:dateAx>
+        <c:axId val="899350543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="44256"/>
+          <c:min val="43976"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-409]mmm\-yy;@" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="899360111"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+        <c:majorUnit val="1"/>
+        <c:majorTimeUnit val="months"/>
+        <c:minorUnit val="1"/>
+        <c:minorTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="899360111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+                  <a:t>Cases (in Millions)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="899350543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.86586040026246736"/>
+          <c:y val="2.4847345373782689E-2"/>
+          <c:w val="7.6499412756373827E-2"/>
+          <c:h val="0.94070513493279595"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
   </c:spPr>
   <c:txPr>
     <a:bodyPr/>
@@ -10055,6 +11853,43 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent4"/>
@@ -12139,6 +13974,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -12400,15 +14740,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>79</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>259978</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>143436</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12430,6 +14770,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>259977</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>161364</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23180720-215B-4894-8F9F-487DD3F98504}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -13537,8 +15915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EBEE6B8-6449-4BD3-9780-821FDD19DB72}">
   <dimension ref="A1:S76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q94" sqref="Q94"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N130" sqref="N130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>